<commit_message>
Add other relevant files
QR Mate setup exe
Screenshots
Logo and Png
</commit_message>
<xml_diff>
--- a/QRMateData/data_source.xlsx
+++ b/QRMateData/data_source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QR Mate Test\QR Mate V1.0-Test 2\QRMateData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swho-shashika\Desktop\QRMateData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Category</t>
   </si>
@@ -36,6 +36,30 @@
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>T-Shirt</t>
+  </si>
+  <si>
+    <t>Polo</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Crew Neck</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Extra large</t>
   </si>
 </sst>
 </file>
@@ -353,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,6 +405,62 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>